<commit_message>
Added to list of papers and changed array system
shifted to haveing having time starting at t=1 in the LP so having the initial S0 storage state would make more sense. Also added to the list of papers in excel document.
</commit_message>
<xml_diff>
--- a/ListOfPapers.xlsx
+++ b/ListOfPapers.xlsx
@@ -24,28 +24,86 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Title</t>
   </si>
   <si>
-    <t>Short Description</t>
-  </si>
-  <si>
     <t>Link</t>
   </si>
   <si>
     <t>Estimating the Maximum Potential Revenue for Grid Connected Electricity Storage: Arbitrage and Regulation</t>
+  </si>
+  <si>
+    <t>A Stochastic Programming Framework for the Valuation of Electricity Storage</t>
+  </si>
+  <si>
+    <t>https://pdfs.semanticscholar.org/4cc3/9daee258877cbff93156781b660043a49b79.pdf</t>
+  </si>
+  <si>
+    <t>https://www.sandia.gov/ess-ssl/publications/SAND2012-3863.pdf</t>
+  </si>
+  <si>
+    <t>Economic viability of energy storage systems based on price arbitrage potential in real-time U.S. electricity markets</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/pii/S0306261913008301</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/pii/S0306261914003651</t>
+  </si>
+  <si>
+    <t>Agent-based model for electricity consumption and storage to evaluate economic viability of tariff arbitrage for residential sector demand response</t>
+  </si>
+  <si>
+    <t>Energy Storage Arbitrage Under Day-Ahead and Real-Time Price Uncertainty</t>
+  </si>
+  <si>
+    <t>https://ieeexplore.ieee.org/abstract/document/7892020</t>
+  </si>
+  <si>
+    <t>https://ieeexplore.ieee.org/abstract/document/7457714</t>
+  </si>
+  <si>
+    <t>Strategic Sizing of Energy Storage Facilities in Electricity Markets</t>
+  </si>
+  <si>
+    <t>https://economics.mit.edu/files/18357</t>
+  </si>
+  <si>
+    <t>Economics of Grid-Scale Energy Storage</t>
+  </si>
+  <si>
+    <t>https://ieeexplore.ieee.org/document/7562406</t>
+  </si>
+  <si>
+    <t>Optimal Operation of Energy Storage Systems Considering Forecasts and Battery Degradation</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -68,16 +126,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -356,35 +420,98 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="57.5703125" customWidth="1"/>
-    <col min="2" max="3" width="45.7109375" customWidth="1"/>
+    <col min="2" max="2" width="45.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+    </row>
+    <row r="2" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="B2" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="B3" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>16</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B3" r:id="rId1"/>
+    <hyperlink ref="B2" r:id="rId2"/>
+    <hyperlink ref="B8" r:id="rId3"/>
+    <hyperlink ref="B9" r:id="rId4"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Included additional conditional constraints
</commit_message>
<xml_diff>
--- a/ListOfPapers.xlsx
+++ b/ListOfPapers.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Title</t>
   </si>
@@ -78,6 +78,12 @@
   </si>
   <si>
     <t>Optimal Operation of Energy Storage Systems Considering Forecasts and Battery Degradation</t>
+  </si>
+  <si>
+    <t>The Importance of Temporal Resolution in Evaluating Residential Energy Storage</t>
+  </si>
+  <si>
+    <t>https://ieeexplore.ieee.org/stamp/stamp.jsp?tp=&amp;arnumber=8274019&amp;tag=1</t>
   </si>
 </sst>
 </file>
@@ -420,7 +426,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A11" sqref="A11"/>
@@ -473,7 +479,7 @@
       </c>
     </row>
     <row r="6" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -481,7 +487,7 @@
       </c>
     </row>
     <row r="7" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="A7" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B7" s="1" t="s">
@@ -489,19 +495,27 @@
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="A8" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+    <row r="9" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -510,6 +524,7 @@
     <hyperlink ref="B2" r:id="rId2"/>
     <hyperlink ref="B8" r:id="rId3"/>
     <hyperlink ref="B9" r:id="rId4"/>
+    <hyperlink ref="B10" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>